<commit_message>
new sites and csv files
</commit_message>
<xml_diff>
--- a/_data/sites.xlsx
+++ b/_data/sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adbrett/Documents/GitHub/orange76xyz/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE4D3E14-1C95-B442-9F09-5AD52FC43719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08F2046-0400-1946-B673-4F044072EA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="2300" windowWidth="23220" windowHeight="15700" xr2:uid="{72CE27DD-7498-EC40-96F8-DE8D241D95D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="147">
   <si>
     <t>Name</t>
   </si>
@@ -50,46 +50,7 @@
     <t>feed</t>
   </si>
   <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>affecognitive ~ religion, film, affect, academia</t>
-  </si>
-  <si>
-    <t>https://affecognitive.wordpress.com/</t>
-  </si>
-  <si>
     <t>/images/sites/affecognitive.jpg</t>
-  </si>
-  <si>
-    <t>https://affecognitive.wordpress.com/feed</t>
-  </si>
-  <si>
-    <t>blog</t>
-  </si>
-  <si>
-    <t>American Indian Law Alliance</t>
-  </si>
-  <si>
-    <t>https://aila.ngo/</t>
-  </si>
-  <si>
-    <t>/images/sites/aila.png</t>
-  </si>
-  <si>
-    <t>https://aila.ngo/feed/</t>
-  </si>
-  <si>
-    <t>An und für sich</t>
-  </si>
-  <si>
-    <t>https://itself.blog/</t>
-  </si>
-  <si>
-    <t>/images/sites/itself.jpg</t>
-  </si>
-  <si>
-    <t>https://itself.blog/feed/</t>
   </si>
   <si>
     <t>Andrew Whitehead</t>
@@ -942,15 +903,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93C3EE4-7221-C946-A74D-D9CE8D794EBB}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E40"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -963,690 +924,532 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="2" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="C11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="D11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="2" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="B12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="2" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="B13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="4" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="2" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="D16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="2" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="B17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="4" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="D18" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="2" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C19" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D19" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="2" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="B20" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="2" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="2" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="4" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C23" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="2" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D24" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="2" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C25" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="2" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="2" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="4" t="s">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D28" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D27" s="2" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="2" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="B30" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D29" s="2" t="s">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D30" s="2" t="s">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D31" s="2" t="s">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C33" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D32" s="2" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="B34" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D33" s="2" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D34" s="2" t="s">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C36" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D35" s="2" t="s">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="C37" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D36" s="2" t="s">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D38" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" xr:uid="{FACFF84E-40DD-694B-9C5A-63431F4EBE55}"/>
-    <hyperlink ref="B32" r:id="rId2" xr:uid="{CA425142-A58E-D24B-961E-55509901E933}"/>
-    <hyperlink ref="D40" r:id="rId3" xr:uid="{97BC4210-3FAF-CF42-ABC7-D0AF56284EEC}"/>
-    <hyperlink ref="D21" r:id="rId4" xr:uid="{DFEFADFE-CE0D-D648-8FE3-EEEE35B3BB47}"/>
-    <hyperlink ref="D26" r:id="rId5" xr:uid="{C9E87E06-44A5-0945-8AEF-25DEABA7EA1D}"/>
-    <hyperlink ref="D5" r:id="rId6" xr:uid="{7EC351B2-867B-544E-A5B3-054D65A1F8DB}"/>
-    <hyperlink ref="D4" r:id="rId7" xr:uid="{EC9DAFD7-8574-104B-B7EA-D3CEA1BAFA94}"/>
-    <hyperlink ref="B22" r:id="rId8" xr:uid="{5358E928-BB19-6E49-A5BB-932BFE72E9A7}"/>
-    <hyperlink ref="D2" r:id="rId9" xr:uid="{414EF383-F296-994A-AAE1-987AB93A2D70}"/>
-    <hyperlink ref="B5" r:id="rId10" xr:uid="{E77640BC-30BA-A44F-A8CA-5C067CF8ED8E}"/>
-    <hyperlink ref="B6" r:id="rId11" xr:uid="{71CD5FBE-AFBD-EC4C-AA59-833EFBF68F6D}"/>
-    <hyperlink ref="B13" r:id="rId12" xr:uid="{3F989883-6207-774E-90A7-F244493C996E}"/>
-    <hyperlink ref="B17" r:id="rId13" xr:uid="{68E13808-F7A1-9649-A573-3DC6C2E70F94}"/>
-    <hyperlink ref="B18" r:id="rId14" xr:uid="{D66C2EF4-FF73-4344-84CC-638BE081EA77}"/>
-    <hyperlink ref="B36" r:id="rId15" xr:uid="{45311776-407F-E44A-B356-7631878A73FA}"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{FACFF84E-40DD-694B-9C5A-63431F4EBE55}"/>
+    <hyperlink ref="B30" r:id="rId2" xr:uid="{CA425142-A58E-D24B-961E-55509901E933}"/>
+    <hyperlink ref="D38" r:id="rId3" xr:uid="{97BC4210-3FAF-CF42-ABC7-D0AF56284EEC}"/>
+    <hyperlink ref="D19" r:id="rId4" xr:uid="{DFEFADFE-CE0D-D648-8FE3-EEEE35B3BB47}"/>
+    <hyperlink ref="D24" r:id="rId5" xr:uid="{C9E87E06-44A5-0945-8AEF-25DEABA7EA1D}"/>
+    <hyperlink ref="D3" r:id="rId6" xr:uid="{7EC351B2-867B-544E-A5B3-054D65A1F8DB}"/>
+    <hyperlink ref="B20" r:id="rId7" xr:uid="{5358E928-BB19-6E49-A5BB-932BFE72E9A7}"/>
+    <hyperlink ref="B3" r:id="rId8" xr:uid="{E77640BC-30BA-A44F-A8CA-5C067CF8ED8E}"/>
+    <hyperlink ref="B4" r:id="rId9" xr:uid="{71CD5FBE-AFBD-EC4C-AA59-833EFBF68F6D}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{3F989883-6207-774E-90A7-F244493C996E}"/>
+    <hyperlink ref="B15" r:id="rId11" xr:uid="{68E13808-F7A1-9649-A573-3DC6C2E70F94}"/>
+    <hyperlink ref="B16" r:id="rId12" xr:uid="{D66C2EF4-FF73-4344-84CC-638BE081EA77}"/>
+    <hyperlink ref="B34" r:id="rId13" xr:uid="{45311776-407F-E44A-B356-7631878A73FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>